<commit_message>
updated getTimeWeightedCapital() so that it does not include coupon payment anymore
</commit_message>
<xml_diff>
--- a/samples/cash ledger excel 2020-01.xlsx
+++ b/samples/cash ledger excel 2020-01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\geneva\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\geneva\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F933C6D-30BF-400E-B568-6A9A44B79025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97A6D39-6863-45E2-96F3-6B969C4E674A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Cash Ledger - 12XXXChina" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="65">
   <si>
     <t>Currency_OpeningBalDesc</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>Maturity (Interest)</t>
+  </si>
+  <si>
+    <t>Maturity only</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -1032,27 +1038,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U70"/>
+  <dimension ref="A1:U72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M69" sqref="M69"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P73" sqref="P73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1123,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1180,7 +1186,7 @@
       </c>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1243,7 +1249,7 @@
       </c>
       <c r="U3" s="3"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1306,7 +1312,7 @@
       </c>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1369,7 +1375,7 @@
       </c>
       <c r="U5" s="3"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1432,7 +1438,7 @@
       </c>
       <c r="U6" s="3"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1495,7 +1501,7 @@
       </c>
       <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1558,7 +1564,7 @@
       </c>
       <c r="U8" s="3"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1621,7 +1627,7 @@
       </c>
       <c r="U9" s="3"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1684,7 +1690,7 @@
       </c>
       <c r="U10" s="3"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1747,7 +1753,7 @@
       </c>
       <c r="U11" s="3"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1810,7 +1816,7 @@
       </c>
       <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1873,7 +1879,7 @@
       </c>
       <c r="U13" s="3"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1936,7 +1942,7 @@
       </c>
       <c r="U14" s="3"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2002,7 +2008,7 @@
         <v>10785557.121643838</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2065,7 +2071,7 @@
       </c>
       <c r="U16" s="3"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2128,7 +2134,7 @@
       </c>
       <c r="U17" s="3"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2191,7 +2197,7 @@
       </c>
       <c r="U18" s="3"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2257,7 +2263,7 @@
         <v>1018040.0942739727</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2320,7 +2326,7 @@
       </c>
       <c r="U20" s="3"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2383,7 +2389,7 @@
       </c>
       <c r="U21" s="3"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2446,7 +2452,7 @@
       </c>
       <c r="U22" s="3"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2509,7 +2515,7 @@
       </c>
       <c r="U23" s="3"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2572,7 +2578,7 @@
       </c>
       <c r="U24" s="3"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2638,7 +2644,7 @@
         <v>20215206.930630136</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2701,7 +2707,7 @@
       </c>
       <c r="U26" s="3"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2764,7 +2770,7 @@
       </c>
       <c r="U27" s="3"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2827,7 +2833,7 @@
       </c>
       <c r="U28" s="3"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -2890,7 +2896,7 @@
       </c>
       <c r="U29" s="3"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2953,7 +2959,7 @@
       </c>
       <c r="U30" s="3"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -3016,7 +3022,7 @@
       </c>
       <c r="U31" s="3"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -3079,7 +3085,7 @@
       </c>
       <c r="U32" s="3"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -3142,7 +3148,7 @@
       </c>
       <c r="U33" s="3"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -3205,7 +3211,7 @@
       </c>
       <c r="U34" s="3"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -3268,7 +3274,7 @@
       </c>
       <c r="U35" s="3"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -3331,7 +3337,7 @@
       </c>
       <c r="U36" s="3"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -3394,7 +3400,7 @@
       </c>
       <c r="U37" s="3"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -3457,7 +3463,7 @@
       </c>
       <c r="U38" s="3"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -3520,7 +3526,7 @@
       </c>
       <c r="U39" s="3"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -3583,7 +3589,7 @@
       </c>
       <c r="U40" s="3"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -3646,7 +3652,7 @@
       </c>
       <c r="U41" s="3"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -3709,7 +3715,7 @@
       </c>
       <c r="U42" s="3"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -3772,7 +3778,7 @@
       </c>
       <c r="U43" s="3"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -3835,7 +3841,7 @@
       </c>
       <c r="U44" s="3"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -3898,7 +3904,7 @@
       </c>
       <c r="U45" s="3"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -3961,7 +3967,7 @@
       </c>
       <c r="U46" s="3"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -4024,7 +4030,7 @@
       </c>
       <c r="U47" s="3"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -4090,7 +4096,7 @@
         <v>31938082.19178082</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -4153,7 +4159,7 @@
       </c>
       <c r="U49" s="3"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -4216,7 +4222,7 @@
       </c>
       <c r="U50" s="3"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -4279,7 +4285,7 @@
       </c>
       <c r="U51" s="3"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -4342,7 +4348,7 @@
       </c>
       <c r="U52" s="3"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -4405,7 +4411,7 @@
       </c>
       <c r="U53" s="3"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -4468,7 +4474,7 @@
       </c>
       <c r="U54" s="3"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>26</v>
       </c>
@@ -4531,7 +4537,7 @@
       </c>
       <c r="U55" s="3"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -4594,7 +4600,7 @@
       </c>
       <c r="U56" s="3"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>26</v>
       </c>
@@ -4657,7 +4663,7 @@
       </c>
       <c r="U57" s="3"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -4720,7 +4726,7 @@
       </c>
       <c r="U58" s="3"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -4783,7 +4789,7 @@
       </c>
       <c r="U59" s="3"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -4846,7 +4852,7 @@
       </c>
       <c r="U60" s="3"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -4909,7 +4915,7 @@
       </c>
       <c r="U61" s="3"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -4972,7 +4978,7 @@
       </c>
       <c r="U62" s="3"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -5035,7 +5041,7 @@
       </c>
       <c r="U63" s="3"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -5098,7 +5104,7 @@
       </c>
       <c r="U64" s="3"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -5161,7 +5167,7 @@
       </c>
       <c r="U65" s="3"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>26</v>
       </c>
@@ -5224,7 +5230,7 @@
       </c>
       <c r="U66" s="3"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -5287,15 +5293,18 @@
       </c>
       <c r="U67" s="3"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I68" t="s">
         <v>62</v>
       </c>
       <c r="K68" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M68" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E69" t="s">
         <v>57</v>
       </c>
@@ -5315,12 +5324,27 @@
         <v>186332788.70238355</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E70" t="s">
         <v>58</v>
       </c>
       <c r="G70" s="1">
         <v>43890</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="I71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="I72" s="3">
+        <f>S9+S32+S34+S35+S36+S64+S67</f>
+        <v>99965701.416438356</v>
+      </c>
+      <c r="M72" s="3">
+        <f>I72+K69</f>
+        <v>163922587.75476712</v>
       </c>
     </row>
   </sheetData>

</xml_diff>